<commit_message>
Added pages, deleted topic areas
</commit_message>
<xml_diff>
--- a/_site/Data/Historical.xlsx
+++ b/_site/Data/Historical.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B40255D-A1E4-DC4B-952B-EA77BC2F404D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85486E3E-7656-4243-A904-14E970858AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16200" xr2:uid="{663F1AFD-6E9B-E447-A23D-DE2FC8DC025F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t xml:space="preserve">What is your ethnicity? </t>
   </si>
@@ -44,6 +44,75 @@
   </si>
   <si>
     <t>Question:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior to coronavirus (COVID-19), did you get free or reduced lunches for your child(ren)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Yes, my child(ren) received free or reduced lunches  
+• No, my child did not receive free or reduced lunches, but they were available 
+• No, free or reduced lunches were not available for my children  
+• No, but I had planned on getting free or reduced lunches for my children soon  
+• No, I didn't know how to access this resource 
+• Not applicable </t>
+  </si>
+  <si>
+    <t>Meet Basic Needs for Health and Well-Being</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you currently get free or reduced lunches for your child(ren)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Yes, my child(ren) receive(s) free or reduced lunches  
+• No, my child does not receive free or reduced lunches, but they were available 
+• No, free or reduced lunches are not available for my children  
+• No, but I plan on getting free or reduced lunches for my children soon  
+• No, I don't know how to access this resource 
+• Not applicable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the past month, how hard has it been for you to pay for the very basics like food, housing, medical care, and heating? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Very hard 
+• Hard 
+• Somewhat hard  
+• Not very hard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of these needs have been hard to pay for in the past month? Select all that apply.  </t>
+  </si>
+  <si>
+    <t>• Food 
+• Housing 
+• Utilities (electric, water, trash) 
+• Healthcare 
+• Social 
+• Emotional 
+• Childcare 
+• Other (please specify) [text entry] 
+• None of the above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What are the biggest challenges and concerns for you and your family right now? </t>
+  </si>
+  <si>
+    <t>Open answer</t>
+  </si>
+  <si>
+    <t>Open Ended Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is helping you and your family the most right now? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is on your mind the most when you think about your community re-opening? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">What concerns do you have about your place of employment and/or your child’s child care setting re-opening? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is there anything else you would like to tell us about you and your family’s experiences during the COVID-19 pandemic? </t>
   </si>
 </sst>
 </file>
@@ -401,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AAEF64-5CC6-0C4E-8EBE-181A98472300}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -432,6 +501,135 @@
       </c>
       <c r="C2" s="2"/>
     </row>
+    <row r="3" spans="1:4" ht="409.6">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="409.6">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="204">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="306">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="136">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="102">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="153">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="187">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="204">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>